<commit_message>
Update Pending Tasks & Projects.xlsx
</commit_message>
<xml_diff>
--- a/Pending Tasks & Projects.xlsx
+++ b/Pending Tasks & Projects.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9BB2E3-5491-45D9-A4C7-FE0EAE767345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Software" sheetId="9" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -189,11 +188,14 @@
   <si>
     <t>Drawing need to prepare for LCD &amp; Backlite after finalizing, Pending Inputs from marketting</t>
   </si>
+  <si>
+    <t>Inform field failure to Pratik</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -405,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,6 +542,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -831,14 +836,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -858,14 +863,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -903,7 +908,7 @@
       <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="53" t="s">
         <v>25</v>
       </c>
     </row>
@@ -923,7 +928,7 @@
       <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
@@ -941,7 +946,7 @@
       <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
@@ -959,17 +964,17 @@
       <c r="E6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="54"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1042,11 +1047,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,16 +1067,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1268,6 +1273,28 @@
         <v>45221</v>
       </c>
       <c r="H9" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49">
+        <v>8</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="40" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1281,7 +1308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">

</xml_diff>